<commit_message>
kevytkoris su 10-12 Maininki
</commit_message>
<xml_diff>
--- a/Poikkeusvuorot vko11.xlsx
+++ b/Poikkeusvuorot vko11.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="118">
   <si>
     <t>VAKIOVUOROT 2021-23</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>10.00-12.00</t>
+  </si>
+  <si>
+    <t>Kevytkoris</t>
   </si>
   <si>
     <t>18.30-20.00</t>
@@ -521,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -586,6 +589,9 @@
     </xf>
     <xf borderId="1" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1158,7 +1164,9 @@
       <c r="N8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="12"/>
+      <c r="O8" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
@@ -1174,37 +1182,37 @@
     <row r="9">
       <c r="A9" s="10"/>
       <c r="B9" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O9" s="12"/>
       <c r="P9" s="9"/>
@@ -1222,19 +1230,19 @@
     <row r="10">
       <c r="A10" s="10"/>
       <c r="B10" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="F10" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>37</v>
@@ -1244,11 +1252,11 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="9"/>
@@ -1276,14 +1284,14 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
@@ -1327,7 +1335,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>38</v>
@@ -1338,7 +1346,7 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="16" t="s">
@@ -1346,17 +1354,17 @@
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K13" s="17"/>
       <c r="L13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="23"/>
+      <c r="M13" s="24"/>
       <c r="N13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O13" s="24"/>
+      <c r="O13" s="25"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
@@ -1372,33 +1380,33 @@
     <row r="14">
       <c r="A14" s="10"/>
       <c r="B14" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
-      <c r="M14" s="23"/>
+      <c r="M14" s="24"/>
       <c r="N14" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
-      <c r="O14" s="24"/>
+      <c r="O14" s="25"/>
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
@@ -1418,23 +1426,23 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
-      <c r="M15" s="25"/>
+      <c r="M15" s="26"/>
       <c r="N15" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
-      <c r="O15" s="24"/>
+      <c r="O15" s="25"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
@@ -1460,13 +1468,13 @@
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
-      <c r="M16" s="25"/>
+      <c r="M16" s="26"/>
       <c r="N16" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
-      <c r="O16" s="24"/>
+      <c r="O16" s="25"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
@@ -1492,13 +1500,13 @@
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
-      <c r="M17" s="25"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
-      <c r="O17" s="24"/>
+      <c r="O17" s="25"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
@@ -1569,19 +1577,19 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
-      <c r="E20" s="26" t="s">
-        <v>66</v>
+      <c r="E20" s="27" t="s">
+        <v>67</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1592,10 +1600,10 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O20" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
@@ -1612,10 +1620,10 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1727,7 +1735,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>36</v>
@@ -1744,11 +1752,11 @@
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
       <c r="L25" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="9"/>
@@ -1766,13 +1774,13 @@
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="6"/>
@@ -1780,11 +1788,11 @@
       <c r="J26" s="17"/>
       <c r="K26" s="7"/>
       <c r="L26" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O26" s="12"/>
       <c r="P26" s="9"/>
@@ -1802,13 +1810,13 @@
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="6"/>
@@ -1816,11 +1824,11 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M27" s="11"/>
       <c r="N27" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O27" s="12"/>
       <c r="P27" s="9"/>
@@ -1893,7 +1901,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1903,21 +1911,21 @@
         <v>34</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
       <c r="J30" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -1940,18 +1948,18 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
       <c r="J31" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
@@ -1976,10 +1984,10 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -2058,25 +2066,25 @@
       <c r="Z34" s="9"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="27" t="s">
-        <v>79</v>
+      <c r="A35" s="28" t="s">
+        <v>80</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="29" t="s">
         <v>40</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
-      <c r="E35" s="26" t="s">
-        <v>81</v>
+      <c r="E35" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>40</v>
@@ -2085,19 +2093,19 @@
         <v>38</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L35" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M35" s="22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
@@ -2114,39 +2122,39 @@
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="29" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>81</v>
+      <c r="E36" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L36" s="22" t="s">
         <v>41</v>
       </c>
       <c r="M36" s="22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
-      <c r="N36" s="29" t="s">
-        <v>89</v>
+      <c r="N36" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="O36" s="18" t="s">
         <v>40</v>
@@ -2170,25 +2178,25 @@
       <c r="D37" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="26" t="s">
-        <v>81</v>
+      <c r="E37" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="5"/>
       <c r="H37" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K37" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L37" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="5"/>
@@ -2263,31 +2271,31 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>75</v>
+      <c r="E40" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M40" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N40" s="12"/>
       <c r="O40" s="12"/>
@@ -2308,18 +2316,18 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
-      <c r="E41" s="26" t="s">
-        <v>75</v>
+      <c r="E41" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -2397,7 +2405,7 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2413,13 +2421,13 @@
         <v>41</v>
       </c>
       <c r="M44" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
@@ -2446,10 +2454,10 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M45" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N45" s="12"/>
       <c r="O45" s="12"/>
@@ -2467,7 +2475,7 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2476,10 +2484,10 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -2508,10 +2516,10 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J47" s="17"/>
       <c r="K47" s="7"/>
@@ -2561,13 +2569,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="28" t="s">
-        <v>87</v>
+      <c r="B49" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>88</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -2651,7 +2659,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2660,16 +2668,16 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I52" s="20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J52" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
@@ -2698,7 +2706,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>35</v>
@@ -2748,14 +2756,14 @@
       <c r="Z54" s="9"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="27" t="s">
-        <v>104</v>
+      <c r="A55" s="28" t="s">
+        <v>105</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="28" t="s">
-        <v>66</v>
+      <c r="C55" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -2769,13 +2777,13 @@
         <v>41</v>
       </c>
       <c r="M55" s="22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O55" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P55" s="9"/>
       <c r="Q55" s="9"/>
@@ -2792,10 +2800,10 @@
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
-      <c r="C56" s="28" t="s">
-        <v>66</v>
+      <c r="C56" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -2851,29 +2859,29 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="5"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="J58" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
@@ -2894,16 +2902,16 @@
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="10"/>
       <c r="B59" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
-      <c r="E59" s="26" t="s">
-        <v>111</v>
+      <c r="E59" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
@@ -2928,7 +2936,7 @@
       <c r="Z59" s="9"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="30"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="4"/>
@@ -2957,19 +2965,19 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C61" s="28" t="s">
         <v>114</v>
       </c>
+      <c r="C61" s="29" t="s">
+        <v>115</v>
+      </c>
       <c r="D61" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -2996,12 +3004,12 @@
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="10"/>
       <c r="B62" s="3"/>
-      <c r="C62" s="28"/>
+      <c r="C62" s="29"/>
       <c r="D62" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>

</xml_diff>